<commit_message>
Se realizo el taller #1
</commit_message>
<xml_diff>
--- a/taller 1.xlsx
+++ b/taller 1.xlsx
@@ -1,26 +1,165 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\OneDrive\Documentos\UAM\SEMESTRE #6\Bases De Datos 2\Talleres\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0972099A-398F-4680-9F43-DA98549DA328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+  <si>
+    <t>Licencia</t>
+  </si>
+  <si>
+    <t>Rendimiento</t>
+  </si>
+  <si>
+    <t>Escalabilidad</t>
+  </si>
+  <si>
+    <t>Caracteristicas</t>
+  </si>
+  <si>
+    <t>Comunidad</t>
+  </si>
+  <si>
+    <t>Integracion</t>
+  </si>
+  <si>
+    <t>Uso Tipico</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>OracleDataBase</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>GPL (General Public License) para la edición comunitaria, y licencia comercial para la edición empresarial.</t>
+  </si>
+  <si>
+    <t>Licencia comercial propietaria de Oracle.</t>
+  </si>
+  <si>
+    <t>PostgreSQL License, que es una licencia permisiva similar a la licencia MIT.</t>
+  </si>
+  <si>
+    <t>Licencia comercial propietaria de Microsoft.</t>
+  </si>
+  <si>
+    <t>Alto rendimiento en lectura. Puede tener limitaciones en escritura intensiva. Eficiente en consultas simples.</t>
+  </si>
+  <si>
+    <t>Rendimiento excepcional en grandes empresas. Optimizado para grandes volúmenes de datos. Alta eficiencia en operaciones complejas.</t>
+  </si>
+  <si>
+    <t>Rendimiento equilibrado entre lectura y escritura. Excelente en operaciones concurrentes. Soporta cargas de trabajo mixtas.</t>
+  </si>
+  <si>
+    <t>Rendimiento sólido y estable. Optimizado para entornos corporativos con alta carga. Buen manejo de consultas complejas.</t>
+  </si>
+  <si>
+    <t>Escalable horizontalmente con particionamiento y replicación. Escalabilidad limitada en entornos extremadamente grandes. Ideal para aplicaciones web de rápido crecimiento.</t>
+  </si>
+  <si>
+    <t>Muy escalable, soporta enormes volúmenes de datos. Diseñado para cargas transaccionales intensivas. Escalabilidad avanzada con RAC (Real Application Clusters).</t>
+  </si>
+  <si>
+    <t>Altamente escalable con replicación y sharding. Adecuado para entornos de big data. Buen soporte para escalabilidad horizontal.</t>
+  </si>
+  <si>
+    <t>Escalabilidad tanto vertical como horizontal. Características avanzadas de particionamiento. Integrado con Azure para escalabilidad en la nube.</t>
+  </si>
+  <si>
+    <t>Soporta transacciones ACID. Replicación básica. Soporte limitado para características avanzadas. JSON nativo y características NoSQL.</t>
+  </si>
+  <si>
+    <t>Funciones avanzadas como RAC, Data Guard, y seguridad avanzada. Soporte completo para ACID. Herramientas robustas de recuperación ante desastres. Optimización para aplicaciones de misión crítica.</t>
+  </si>
+  <si>
+    <t>Extensible con módulos. JSON y XML nativos. Soporte avanzado para manejo de datos. Excelente en manejos de funciones complejas y personalizadas.</t>
+  </si>
+  <si>
+    <t>Soporte completo de ACID. Seguridad avanzada y cifrado. Particionamiento y replicación integrados. Herramientas avanzadas de análisis y BI (Business Intelligence).</t>
+  </si>
+  <si>
+    <t>Amplia comunidad open source. Bien documentada. Activa en foros y contribuciones. Abundancia de tutoriales y recursos educativos.</t>
+  </si>
+  <si>
+    <t>Comunidad cerrada. Dependencia del soporte de Oracle. Recursos limitados fuera del ecosistema Oracle. Mayor enfoque en clientes corporativos.</t>
+  </si>
+  <si>
+    <t>Fuerte comunidad open source. Colaborativa y con abundante documentación. Proyectos y extensiones mantenidos activamente. Comunidad global y accesible.</t>
+  </si>
+  <si>
+    <t>Comunidad activa pero dirigida por Microsoft. Soporte profesional disponible. Recursos educativos de alta calidad. Orientada a clientes corporativos.</t>
+  </si>
+  <si>
+    <t>Amplia integración con diversas tecnologías. Compatible con múltiples lenguajes de programación. Fácil de integrar en entornos de desarrollo web. Herramientas de terceros disponibles.</t>
+  </si>
+  <si>
+    <t>Integración profunda con tecnologías Oracle. Integración nativa con herramientas empresariales de Oracle. Optimizado para ecosistemas corporativos. Compatible con ERP y CRM de Oracle.</t>
+  </si>
+  <si>
+    <t>Excelente integración con múltiples plataformas. Soporte para JSON y NoSQL. Compatible con una amplia gama de tecnologías y lenguajes. Fácil de integrar en aplicaciones heterogéneas.</t>
+  </si>
+  <si>
+    <t>Integración nativa con productos Microsoft. Conexión directa con Azure y Power BI. Compatible con muchas herramientas empresariales. Buena integración con aplicaciones de análisis de datos.</t>
+  </si>
+  <si>
+    <t>Aplicaciones web pequeñas y medianas. Startups y proyectos ágiles. CMS como WordPress, Drupal. Aplicaciones de comercio electrónico.</t>
+  </si>
+  <si>
+    <t>Grandes empresas y corporaciones. Aplicaciones de misión crítica (ERP, CRM). Gestión de grandes bases de datos. Sectores financieros y gubernamentales.</t>
+  </si>
+  <si>
+    <t>Aplicaciones web y móviles. Big data y análisis de datos. Sistemas financieros y empresariales. Desarrollo de software open source.</t>
+  </si>
+  <si>
+    <t>Grandes corporaciones. Aplicaciones empresariales y análisis de datos. BI (Business Intelligence) y reportes. Integración con soluciones Microsoft.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +167,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +212,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +530,158 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.109375" style="2" customWidth="1"/>
+    <col min="6" max="12" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificacion del taller 1
</commit_message>
<xml_diff>
--- a/taller 1.xlsx
+++ b/taller 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\OneDrive\Documentos\UAM\SEMESTRE #6\Bases De Datos 2\Talleres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0972099A-398F-4680-9F43-DA98549DA328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB160784-3C95-4F17-9574-21B1EF49D02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,18 +131,6 @@
     <t>Comunidad activa pero dirigida por Microsoft. Soporte profesional disponible. Recursos educativos de alta calidad. Orientada a clientes corporativos.</t>
   </si>
   <si>
-    <t>Amplia integración con diversas tecnologías. Compatible con múltiples lenguajes de programación. Fácil de integrar en entornos de desarrollo web. Herramientas de terceros disponibles.</t>
-  </si>
-  <si>
-    <t>Integración profunda con tecnologías Oracle. Integración nativa con herramientas empresariales de Oracle. Optimizado para ecosistemas corporativos. Compatible con ERP y CRM de Oracle.</t>
-  </si>
-  <si>
-    <t>Excelente integración con múltiples plataformas. Soporte para JSON y NoSQL. Compatible con una amplia gama de tecnologías y lenguajes. Fácil de integrar en aplicaciones heterogéneas.</t>
-  </si>
-  <si>
-    <t>Integración nativa con productos Microsoft. Conexión directa con Azure y Power BI. Compatible con muchas herramientas empresariales. Buena integración con aplicaciones de análisis de datos.</t>
-  </si>
-  <si>
     <t>Aplicaciones web pequeñas y medianas. Startups y proyectos ágiles. CMS como WordPress, Drupal. Aplicaciones de comercio electrónico.</t>
   </si>
   <si>
@@ -153,6 +141,18 @@
   </si>
   <si>
     <t>Grandes corporaciones. Aplicaciones empresariales y análisis de datos. BI (Business Intelligence) y reportes. Integración con soluciones Microsoft.</t>
+  </si>
+  <si>
+    <t>Amplia integración con diversas tecnologías. Compatible con múltiples lenguajes de programación: PHP, Python, Java, Ruby, C, C++, Perl. Fácil de integrar en entornos de desarrollo web. Herramientas de terceros disponibles.</t>
+  </si>
+  <si>
+    <t>Integración profunda con tecnologías Oracle. Integración nativa con herramientas empresariales de Oracle. Fuertemente integrado con Java, PL/SQL, C, C++. Optimizado para ecosistemas corporativos. Compatible con ERP y CRM de Oracle.</t>
+  </si>
+  <si>
+    <t>Excelente integración con múltiples plataformas. Soporte para JSON y NoSQL. Compatible con una amplia gama de tecnologías y lenguajes: Python, Java, Ruby, Go, C, C++, Perl. Fácil de integrar en aplicaciones heterogéneas.</t>
+  </si>
+  <si>
+    <t>Integración nativa con productos Microsoft. Fuertemente integrado con .NET, C#, Java, Python, R, Visual Basic. Conexión directa con Azure y Power BI. Compatible con muchas herramientas empresariales. Buena integración con aplicaciones de análisis de datos.</t>
   </si>
 </sst>
 </file>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,21 +647,21 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="57" customHeight="1" x14ac:dyDescent="0.3">
@@ -669,16 +669,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>